<commit_message>
added ft # and starting #
</commit_message>
<xml_diff>
--- a/Excel/demo (2).xlsx
+++ b/Excel/demo (2).xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:D21"/>
+  <dimension ref="A3:D61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -724,6 +724,490 @@
         <v>0.42619788646698</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Num</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D23" s="1" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1</v>
+      </c>
+      <c r="B24" t="n">
+        <v>8.402608871459961</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.6628193855285645</v>
+      </c>
+      <c r="D24" t="n">
+        <v>7.739789485931396</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2</v>
+      </c>
+      <c r="B25" t="n">
+        <v>8.299276351928711</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.7217079997062683</v>
+      </c>
+      <c r="D25" t="n">
+        <v>7.577568531036377</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>3</v>
+      </c>
+      <c r="B26" t="n">
+        <v>8.402608871459961</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.6619071364402771</v>
+      </c>
+      <c r="D26" t="n">
+        <v>7.740701675415039</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>Num</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D28" s="1" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1</v>
+      </c>
+      <c r="B29" t="n">
+        <v>8.402608871459961</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.6563481092453003</v>
+      </c>
+      <c r="D29" t="n">
+        <v>7.746260643005371</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2</v>
+      </c>
+      <c r="B30" t="n">
+        <v>8.299276351928711</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.7046168446540833</v>
+      </c>
+      <c r="D30" t="n">
+        <v>7.594659328460693</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>3</v>
+      </c>
+      <c r="B31" t="n">
+        <v>8.402608871459961</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.6621693968772888</v>
+      </c>
+      <c r="D31" t="n">
+        <v>7.740439414978027</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>Num</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D33" s="1" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>1</v>
+      </c>
+      <c r="B34" t="n">
+        <v>8.402608871459961</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.6620481610298157</v>
+      </c>
+      <c r="D34" t="n">
+        <v>7.740560531616211</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2</v>
+      </c>
+      <c r="B35" t="n">
+        <v>8.299276351928711</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.7242947220802307</v>
+      </c>
+      <c r="D35" t="n">
+        <v>7.574981689453125</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>Num</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D37" s="1" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>1</v>
+      </c>
+      <c r="B38" t="n">
+        <v>8.402608871459961</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.6635361313819885</v>
+      </c>
+      <c r="D38" t="n">
+        <v>7.739072799682617</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>6</v>
+      </c>
+      <c r="B39" t="n">
+        <v>3.814814567565918</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.9300078749656677</v>
+      </c>
+      <c r="D39" t="n">
+        <v>2.884806632995605</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>13</v>
+      </c>
+      <c r="B40" t="n">
+        <v>8.402608871459961</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.6647151708602905</v>
+      </c>
+      <c r="D40" t="n">
+        <v>7.737893581390381</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>Num</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D42" s="1" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1</v>
+      </c>
+      <c r="B43" t="n">
+        <v>8.402608871459961</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.6621693968772888</v>
+      </c>
+      <c r="D43" t="n">
+        <v>7.740439414978027</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>Num</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D45" s="1" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>1</v>
+      </c>
+      <c r="B46" t="n">
+        <v>8.402608871459961</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.6811108589172363</v>
+      </c>
+      <c r="D46" t="n">
+        <v>7.721498012542725</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>Num</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D48" s="1" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1</v>
+      </c>
+      <c r="B49" t="n">
+        <v>8.402608871459961</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.6569118499755859</v>
+      </c>
+      <c r="D49" t="n">
+        <v>7.745697021484375</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>17</v>
+      </c>
+      <c r="B51" t="n">
+        <v>8.402608871459961</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.6690974235534668</v>
+      </c>
+      <c r="D51" t="n">
+        <v>7.733511447906494</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>Num</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="C53" s="1" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D53" s="1" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>1</v>
+      </c>
+      <c r="B54" t="n">
+        <v>8.402608871459961</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.6624118089675903</v>
+      </c>
+      <c r="D54" t="n">
+        <v>7.74019718170166</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>2</v>
+      </c>
+      <c r="B55" t="n">
+        <v>8.299276351928711</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.7033462524414062</v>
+      </c>
+      <c r="D55" t="n">
+        <v>7.595930099487305</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>3</v>
+      </c>
+      <c r="B56" t="n">
+        <v>7.370575428009033</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.7949501276016235</v>
+      </c>
+      <c r="D56" t="n">
+        <v>6.575625419616699</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>4</v>
+      </c>
+      <c r="B57" t="n">
+        <v>7.817458152770996</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.6562545299530029</v>
+      </c>
+      <c r="D57" t="n">
+        <v>7.161203384399414</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>5</v>
+      </c>
+      <c r="B58" t="n">
+        <v>7.809852600097656</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.9485856294631958</v>
+      </c>
+      <c r="D58" t="n">
+        <v>6.86126708984375</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>4</v>
+      </c>
+      <c r="B59" t="n">
+        <v>8.402608871459961</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.6605494022369385</v>
+      </c>
+      <c r="D59" t="n">
+        <v>7.742059707641602</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>5</v>
+      </c>
+      <c r="B61" t="n">
+        <v>8.299276351928711</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.6904088854789734</v>
+      </c>
+      <c r="D61" t="n">
+        <v>7.608867645263672</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>